<commit_message>
got caught, made new account that will run the code, added logger.py
</commit_message>
<xml_diff>
--- a/bots.xlsx
+++ b/bots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>gmail</t>
   </si>
@@ -59,23 +59,77 @@
     <t>9zwnGkYGVfieUIxJfc6i55vWd3WegFMlSKmK8AsCcpNLI0d3Rw</t>
   </si>
   <si>
-    <t>access key</t>
-  </si>
-  <si>
-    <t>access secret</t>
-  </si>
-  <si>
     <t>885340635854753793-5XDrIQmk1mnoOoslMnnx01k6I74nxOD</t>
   </si>
   <si>
     <t>AqB2R8jCRs9us7cXzIc7jJp8yZYM7ALJxU1XslFDT14OR</t>
+  </si>
+  <si>
+    <t>doodlebob0042</t>
+  </si>
+  <si>
+    <t>dgeg45?12</t>
+  </si>
+  <si>
+    <t>doodlebob0043</t>
+  </si>
+  <si>
+    <t>yahoo</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>wRVSTKYDJWCHFmagYg8qhZQwF</t>
+  </si>
+  <si>
+    <t>zGSRwPz9w3SpPW1XWoyurJMxU1Rqk9vg1vD0dOVw64N8u278Ss</t>
+  </si>
+  <si>
+    <t>890052028675784000aHiBYsLVMFbyWxzvU1oEndDY5Pjx641</t>
+  </si>
+  <si>
+    <t>ZSWgsMuQRFY1zzPjB8HNAWyWFzrBqD69gN2E687NJsP90</t>
+  </si>
+  <si>
+    <t>cougarGuy01</t>
+  </si>
+  <si>
+    <t>meow01</t>
+  </si>
+  <si>
+    <t>application name = cougarGuy01!</t>
+  </si>
+  <si>
+    <t>url = https://na.com</t>
+  </si>
+  <si>
+    <t>MEpbDNplsX724pFmaKtTjlMFW</t>
+  </si>
+  <si>
+    <t>BEIyPrCYzWe8X65fArKE65cXAkLtyUd8RAYlLllHrw4ubiND9T</t>
+  </si>
+  <si>
+    <t>932834480406122497-kEdX6h2yZ7ocWhEgVznG22My7qbeLx5</t>
+  </si>
+  <si>
+    <t>0hjm4BHFfCiHgNwNVccNw66puL0ZN22hwGinrtdjrW2d6</t>
+  </si>
+  <si>
+    <t>access token secret</t>
+  </si>
+  <si>
+    <t>access token</t>
+  </si>
+  <si>
+    <t>bavalley1@cougars.ccis.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +140,12 @@
     <font>
       <sz val="8"/>
       <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -110,10 +170,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,74 +458,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>29221</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>29221</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
+    <row r="3" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="D3" t="s">
         <v>14</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>